<commit_message>
refactor: update main.py to read and print data from Excel file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdullah\Desktop\practice\projects\excel_file_reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDF66E52-51B3-4E45-9317-49ABA2617607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63355DA-F1B8-4241-B1AA-F0AF902510BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{81CB8140-1108-44DB-81F6-ECD31F317284}"/>
   </bookViews>
@@ -34,23 +34,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Abdullah</t>
   </si>
   <si>
-    <t>password</t>
+    <t>Ahmed</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Hassan</t>
+  </si>
+  <si>
+    <t>Umar</t>
+  </si>
+  <si>
+    <t>Bilal</t>
+  </si>
+  <si>
+    <t>Zain</t>
+  </si>
+  <si>
+    <t>Saad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -78,8 +101,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,28 +423,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB7DB79-8C83-4114-A969-B2126E831F3C}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="2">
+        <v>12345788</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>84930211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>12345788</v>
+      <c r="B4" s="2">
+        <v>77219834</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>66549012</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>90871234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>33458790</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>55671209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>78123456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: correct print formatting in main.py for better readability
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdullah\Desktop\practice\projects\excel_file_reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63355DA-F1B8-4241-B1AA-F0AF902510BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC341A5-309D-4ECE-9CB4-181967F9F134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{81CB8140-1108-44DB-81F6-ECD31F317284}"/>
   </bookViews>
@@ -34,9 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>name</t>
+  </si>
   <si>
     <t>Abdullah</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
   <si>
     <t>Ahmed</t>
@@ -426,7 +432,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,12 +442,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>12345788</v>
@@ -449,7 +459,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>84930211</v>
@@ -457,7 +467,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>77219834</v>
@@ -465,7 +475,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>66549012</v>
@@ -473,7 +483,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>90871234</v>
@@ -481,7 +491,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>33458790</v>
@@ -489,7 +499,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>55671209</v>
@@ -497,7 +507,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>78123456</v>

</xml_diff>